<commit_message>
Template cell alignment fix.
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Experiment_run_Infinium_v5_0_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Experiment_run_Infinium_v5_0_0.xlsx
@@ -1855,7 +1855,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1957,10 +1957,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2101,7 +2097,7 @@
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48828125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.49609375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="48.43"/>
@@ -44182,7 +44178,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.49609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="24.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="25.86"/>
@@ -44403,12 +44399,12 @@
       <c r="H18" s="3"/>
       <c r="I18" s="24"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="25"/>
-      <c r="E19" s="26"/>
+      <c r="E19" s="23"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="24"/>
@@ -51586,7 +51582,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="26" t="s">
         <v>62</v>
       </c>
     </row>
@@ -51606,419 +51602,419 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="27" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="23"/>
-      <c r="B8" s="29"/>
+      <c r="B8" s="28"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="B9" s="29"/>
+      <c r="B9" s="28"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="31" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="31" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="31" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="32" t="s">
+      <c r="B13" s="31" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="32" t="s">
+      <c r="B14" s="31" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="31" t="s">
+      <c r="A15" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="31" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="31" t="s">
+      <c r="A16" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="31" t="s">
+      <c r="B16" s="30" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="31" t="s">
+      <c r="A17" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="31" t="s">
+      <c r="B17" s="30" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="31" t="s">
+      <c r="A18" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="31" t="s">
+      <c r="B18" s="30" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="31" t="s">
+      <c r="A19" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="31" t="s">
+      <c r="B19" s="30" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="31" t="s">
+      <c r="A20" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="31" t="s">
+      <c r="B20" s="30" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="31" t="s">
+      <c r="A21" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="31" t="s">
+      <c r="B21" s="30" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="31" t="s">
+      <c r="A22" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="31" t="s">
+      <c r="B22" s="30" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="31" t="s">
+      <c r="A23" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="31" t="s">
+      <c r="B23" s="30" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="31" t="s">
+      <c r="A24" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="31" t="s">
+      <c r="B24" s="30" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="31" t="s">
+      <c r="A25" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="B25" s="31" t="s">
+      <c r="B25" s="30" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="31" t="s">
+      <c r="A26" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="31" t="s">
+      <c r="B26" s="30" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="B27" s="31" t="s">
+      <c r="B27" s="30" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="31" t="s">
+      <c r="A28" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="B28" s="31" t="s">
+      <c r="B28" s="30" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="31" t="s">
+      <c r="A29" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="31" t="s">
+      <c r="B29" s="30" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="31" t="s">
+      <c r="A30" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="B30" s="31" t="s">
+      <c r="B30" s="30" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="31" t="s">
+      <c r="A31" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="31" t="s">
+      <c r="B31" s="30" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="31" t="s">
+      <c r="A32" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="31" t="s">
+      <c r="B32" s="30" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="31" t="s">
+      <c r="A33" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="31" t="s">
+      <c r="B33" s="30" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="31" t="s">
+      <c r="A34" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="B34" s="31" t="s">
+      <c r="B34" s="30" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="31" t="s">
+      <c r="A35" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="B35" s="31" t="s">
+      <c r="B35" s="30" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="31" t="s">
+      <c r="A36" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="B36" s="31" t="s">
+      <c r="B36" s="30" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="31" t="s">
+      <c r="A37" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="B37" s="31" t="s">
+      <c r="B37" s="30" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="31" t="s">
+      <c r="A38" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="B38" s="31" t="s">
+      <c r="B38" s="30" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="31" t="s">
+      <c r="A39" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="B39" s="31" t="s">
+      <c r="B39" s="30" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="31" t="s">
+      <c r="A40" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="B40" s="31" t="s">
+      <c r="B40" s="30" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="31" t="s">
+      <c r="A41" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="B41" s="31" t="s">
+      <c r="B41" s="30" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="31" t="s">
+      <c r="A42" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="B42" s="31" t="s">
+      <c r="B42" s="30" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="31" t="s">
+      <c r="A43" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="B43" s="31" t="s">
+      <c r="B43" s="30" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="31" t="s">
+      <c r="A44" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="B44" s="31" t="s">
+      <c r="B44" s="30" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="31" t="s">
+      <c r="A45" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="B45" s="31" t="s">
+      <c r="B45" s="30" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="31" t="s">
+      <c r="A46" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="B46" s="31" t="s">
+      <c r="B46" s="30" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="31" t="s">
+      <c r="A47" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="B47" s="31" t="s">
+      <c r="B47" s="30" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="31" t="s">
+      <c r="A48" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="B48" s="31" t="s">
+      <c r="B48" s="30" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="31" t="s">
+      <c r="A49" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="B49" s="31" t="s">
+      <c r="B49" s="30" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="33"/>
-      <c r="B50" s="33"/>
+      <c r="A50" s="32"/>
+      <c r="B50" s="32"/>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="34" t="s">
+      <c r="A51" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="B51" s="33"/>
+      <c r="B51" s="32"/>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="31" t="s">
+      <c r="A52" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B52" s="32" t="s">
+      <c r="B52" s="31" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="31" t="s">
+      <c r="A53" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="B53" s="32" t="s">
+      <c r="B53" s="31" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="31" t="s">
+      <c r="A54" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="B54" s="32" t="s">
+      <c r="B54" s="31" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="31" t="s">
+      <c r="A55" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="B55" s="32" t="s">
+      <c r="B55" s="31" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="31" t="s">
+      <c r="A56" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="B56" s="32" t="s">
+      <c r="B56" s="31" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="31" t="s">
+      <c r="A57" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="B57" s="32" t="s">
+      <c r="B57" s="31" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="31" t="s">
+      <c r="A58" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="B58" s="32" t="s">
+      <c r="B58" s="31" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="31" t="s">
+      <c r="A59" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="B59" s="32" t="s">
+      <c r="B59" s="31" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="31" t="s">
+      <c r="A60" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="B60" s="32" t="s">
+      <c r="B60" s="31" t="s">
         <v>83</v>
       </c>
     </row>
@@ -52046,7 +52042,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48828125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.49609375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.43"/>
@@ -52082,10 +52078,10 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="34" t="s">
         <v>91</v>
       </c>
       <c r="C2" s="23" t="s">
@@ -52105,7 +52101,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="34" t="s">
         <v>94</v>
       </c>
       <c r="B3" s="23"/>

</xml_diff>